<commit_message>
Implementation tools update and business processes page
</commit_message>
<xml_diff>
--- a/input/indicators/PNC DAK_indicators.xlsx
+++ b/input/indicators/PNC DAK_indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\PNC DAK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/PNC DAK/_FINAL implementation tools/v0.9.9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084AC704-D319-44DC-A1D4-F559537C34E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{FC8399EC-AA32-44D8-B31A-9575EF62D96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B0C2C0C-57EE-4215-A9FC-1BE65CD8CC61}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <r>
       <t>Digital adaptation kit for</t>
@@ -241,6 +241,77 @@
   </si>
   <si>
     <t>If there are any national or global guidelines (e.g. WHO guidelines) that dictate how and why this indicator should be calculated or reported, they should be noted here. If any guidelines or recommendations change, having a clear reference listed will help in updating or restructuring your data.</t>
+  </si>
+  <si>
+    <t>https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx</t>
+  </si>
+  <si>
+    <t>© World Health Organization 2025. Some rights reserved.</t>
+  </si>
+  <si>
+    <t>This work is available under the Creative Commons Attribution-NonCommercial-ShareAlike 3.0 IGO licence (CC BY-NC-SA 3.0 IGO https://creativecommons.org/%20licenses/by-nc-sa/3.0/igo).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under the terms of this licence, you may copy, redistribute and adapt the work for non-commercial purposes, provided the work is appropriately cited, as indicated below. In any use of this work, there should be no suggestion that WHO endorses any specific organization, products or services. The use of the WHO logo is not permitted. If you adapt the work, then you must license your work under the same or equivalent Creative Commons licence. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Suggested citation. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Digital adaptation kit for postnatal care: operational requirements for implementing WHO recommendations in digital systems. Geneva: World Health Organization; 2025 (SMART Guidelines collection). https://iris.who.int/handle/10665/381725. Licence: CC BY-NC-SA 3.0 IGO.</t>
+    </r>
+  </si>
+  <si>
+    <t>If you create a translation or adaptation of this work, you should add the following disclaimer along with the suggested citation: “This translation/adaptation was not created by the World Health Organization (WHO). WHO is not responsible for the content or accuracy of this translation/adaptation. The original English edition shall be the binding and authentic edition”.</t>
+  </si>
+  <si>
+    <t>If you would like to develop your own Digital Adaptation Kit or create an implementation guide based on this DAK, you can access the SMART Guidelines templates here https://smart.who.int/ig-starter-kit/.</t>
+  </si>
+  <si>
+    <t>Any mediation relating to disputes arising under the licence shall be conducted in accordance with the mediation rules of the World Intellectual Property Organization https://www.wipo.int/amc/en/mediation/rules</t>
+  </si>
+  <si>
+    <t>To submit requests for commercial use and queries on rights and licensing, see https://www.who.int/copyright</t>
+  </si>
+  <si>
+    <r>
+      <t>Third-party materials.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> If you wish to reuse material from this work that is attributed to a third party, such as tables, figures or images, it is your responsibility to determine whether permission is needed for that reuse and to obtain permission from the copyright holder. The risk of claims resulting from infringement of any third-party-owned component in the work rests solely with the user.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>General disclaimers.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The designations employed and the presentation of the material in this publication do not imply the expression of any opinion whatsoever on the part of WHO concerning the legal status of any country, territory, city or area or of its authorities, or concerning the delimitation of its frontiers or boundaries. Dotted and dashed lines on maps represent approximate border lines for which there may not yet be full agreement.</t>
+    </r>
+  </si>
+  <si>
+    <t>The mention of specific companies or of certain manufacturers’ products does not imply that they are endorsed or recommended by WHO in preference to others of a similar nature that are not mentioned. Errors and omissions excepted, the names of proprietary products are distinguished by initial capital letters.</t>
+  </si>
+  <si>
+    <t>All reasonable precautions have been taken by WHO to verify the information contained in this publication. However, the published material is being distributed without warranty of any kind, either expressed or implied. The responsibility for the interpretation and use of the material lies with the reader. In no event shall WHO be liable for damages arising from its use.</t>
   </si>
   <si>
     <t>Indicator ID</t>
@@ -727,9 +798,6 @@
     <t>Short title as referred to in indicator tables</t>
   </si>
   <si>
-    <t>Analysis and use of health facility data: guidance for maternal, newborn, child and adolescent health programme managers (1)</t>
-  </si>
-  <si>
     <r>
       <t>Analysis and use of health facility data: guidance for maternal, newborn, child and adolescent health programme managers. Geneva: World Health Organization; 2023 (</t>
     </r>
@@ -752,6 +820,9 @@
       </rPr>
       <t xml:space="preserve">). </t>
     </r>
+  </si>
+  <si>
+    <t>Analysis and use of health facility data: guidance for maternal, newborn, child and adolescent health programme managers (1)</t>
   </si>
   <si>
     <r>
@@ -820,116 +891,6 @@
       <t>).</t>
     </r>
   </si>
-  <si>
-    <t>https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">© World Health Organization 2025. Some rights reserved.
-This work is available under the Creative Commons Attribution-NonCommercial-ShareAlike 3.0 IGO licence (CC BY-NC-SA 3.0 IGO https://creativecommons.org/%20licenses/by-nc-sa/3.0/igo).
-Under the terms of this licence, you may copy, redistribute and adapt the work for non-commercial purposes, provided the work is appropriately cited, as indicated below. In any use of this work, there should be no suggestion that WHO endorses any specific organization, products or services. The use of the WHO logo is not permitted. If you adapt the work, then you must license your work under the same or equivalent Creative Commons licence. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Suggested citation.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Digital adaptation kit for </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>postnatal care</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: operational requirements for implementing WHO recommendations in digital systems. Geneva: World Health Organization; 2025 (SMART Guidelines collection). </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Insert handle URI]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Licence: CC BY-NC-SA 3.0 IGO. 
-If you create a translation or adaptation of this work, you should add the following disclaimer along with the suggested citation: “This translation/adaptation was not created by the World Health Organization (WHO). WHO is not responsible for the content or accuracy of this translation/adaptation. The original English edition shall be the binding and authentic edition”. 
-If you would like to develop your own Digital Adaptation Kit or create an implementation guide based on this DAK, you can access the SMART Guidelines templates here https://smart.who.int/ig-starter-kit/.
-Any mediation relating to disputes arising under the licence shall be conducted in accordance with the mediation rules of the World Intellectual Property Organization https://www.wipo.int/amc/en/mediation/rules
-To submit requests for commercial use and queries on rights and licensing, see https://www.who.int/copyright
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Third-party materials. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">If you wish to reuse material from this work that is attributed to a third party, such as tables, figures or images, it is your responsibility to determine whether permission is needed for that reuse and to obtain permission from the copyright holder. The risk of claims resulting from infringement of any third-party-owned component in the work rests solely with the user. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>General disclaimers.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> The designations employed and the presentation of the material in this publication do not imply the expression of any opinion whatsoever on the part of WHO concerning the legal status of any country, territory, city or area or of its authorities, or concerning the delimitation of its frontiers or boundaries. Dotted and dashed lines on maps represent approximate border lines for which there may not yet be full agreement. 
-The mention of specific companies or of certain manufacturers’ products does not imply that they are endorsed or recommended by WHO in preference to others of a similar nature that are not mentioned. Errors and omissions excepted, the names of proprietary products are distinguished by initial capital letters. 
-All reasonable precautions have been taken by WHO to verify the information contained in this publication. However, the published material is being distributed without warranty of any kind, either expressed or implied. The responsibility for the interpretation and use of the material lies with the reader. In no event shall WHO be liable for damages arising from its use.</t>
-    </r>
-  </si>
 </sst>
 </file>
 
@@ -938,7 +899,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1179,38 +1140,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1267,6 +1229,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1402,7 +1370,7 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -1412,7 +1380,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -1423,18 +1391,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1442,7 +1410,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1450,10 +1418,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1471,9 +1439,9 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1570,20 +1538,68 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1615,57 +1631,14 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="15" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="16" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -5826,9 +5799,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5866,7 +5839,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5972,7 +5945,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6114,7 +6087,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6125,90 +6098,55 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:K19"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="24.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.453125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="38.81640625" style="57" customWidth="1"/>
-    <col min="5" max="10" width="8.6328125" style="65"/>
-    <col min="11" max="11" width="8.6328125" style="57"/>
-    <col min="12" max="16384" width="8.6328125" style="19"/>
+    <col min="1" max="1" width="4.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="1" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1" ht="89.45" customHeight="1">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="55" t="e" vm="1">
+      <c r="D2" s="34" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="60"/>
     </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1" ht="15">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:11" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+    <row r="4" spans="2:4" s="18" customFormat="1" ht="55.5" customHeight="1">
+      <c r="B4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="62"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
     </row>
-    <row r="5" spans="2:11" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="60"/>
+      <c r="D5" s="19"/>
     </row>
-    <row r="6" spans="2:11" s="1" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="60"/>
+      <c r="D6" s="37"/>
     </row>
-    <row r="7" spans="2:11" s="21" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" s="21" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="B7" s="22" t="s">
         <v>3</v>
       </c>
@@ -6216,15 +6154,8 @@
         <v>4</v>
       </c>
       <c r="D7" s="35"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="58"/>
     </row>
-    <row r="8" spans="2:11" s="21" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" s="21" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="B8" s="22" t="s">
         <v>5</v>
       </c>
@@ -6232,15 +6163,8 @@
         <v>6</v>
       </c>
       <c r="D8" s="35"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="2:11" s="21" customFormat="1" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" s="21" customFormat="1" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
@@ -6248,15 +6172,8 @@
         <v>8</v>
       </c>
       <c r="D9" s="35"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="2:11" s="21" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" s="21" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="B10" s="22" t="s">
         <v>9</v>
       </c>
@@ -6264,31 +6181,17 @@
         <v>10</v>
       </c>
       <c r="D10" s="35"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="2:11" s="21" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" s="21" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="B11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="58"/>
+      <c r="D11" s="39"/>
     </row>
-    <row r="12" spans="2:11" s="21" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4" s="21" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="B12" s="22" t="s">
         <v>13</v>
       </c>
@@ -6296,121 +6199,225 @@
         <v>14</v>
       </c>
       <c r="D12" s="35"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="58"/>
     </row>
-    <row r="13" spans="2:11" s="21" customFormat="1" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" s="21" customFormat="1" ht="35.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="B13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="58"/>
+      <c r="D13" s="38"/>
     </row>
-    <row r="14" spans="2:11" s="21" customFormat="1" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" s="21" customFormat="1" ht="15.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="B14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="58"/>
+      <c r="D14" s="38"/>
     </row>
-    <row r="15" spans="2:11" s="21" customFormat="1" ht="47" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" s="21" customFormat="1" ht="46.9" customHeight="1" thickTop="1" thickBot="1">
       <c r="B15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="58"/>
+      <c r="D15" s="38"/>
     </row>
-    <row r="16" spans="2:11" s="21" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="58"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="58"/>
+    <row r="16" spans="2:4" s="21" customFormat="1" ht="15.75" thickTop="1"/>
+    <row r="17" spans="2:10" s="21" customFormat="1" ht="15">
+      <c r="B17" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
     </row>
-    <row r="17" spans="2:11" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="58"/>
+    <row r="18" spans="2:10" ht="12.75" customHeight="1">
+      <c r="B18" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
-    <row r="18" spans="2:11" s="21" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="58"/>
+    <row r="19" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B19" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
     </row>
-    <row r="19" spans="2:11" s="21" customFormat="1" ht="380" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="58"/>
+    <row r="20" spans="2:10" ht="42" customHeight="1">
+      <c r="B20" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="2:10" ht="27.75" customHeight="1">
+      <c r="B21" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="2:10" ht="48" customHeight="1">
+      <c r="B22" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B23" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="2:10" ht="26.25" customHeight="1">
+      <c r="B24" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="2:10" ht="21" customHeight="1">
+      <c r="B25" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="2:10" ht="42" customHeight="1">
+      <c r="B26" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="2:10" ht="47.25" customHeight="1">
+      <c r="B27" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="2:10" ht="39" customHeight="1">
+      <c r="B28" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="2:10" ht="41.25" customHeight="1">
+      <c r="B29" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="2:10" ht="15">
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="24">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B17:D17"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
@@ -6418,15 +6425,14 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{1A76B07C-04F1-437C-8E9B-E1F4563F44BF}"/>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{B0B72D77-0D0D-4D71-B386-72B5E9B8B90C}"/>
+    <hyperlink ref="B17:D17" r:id="rId2" display="https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx" xr:uid="{4CC2310C-BE7E-4EE3-9A68-9B26A7CF4C01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6439,22 +6445,22 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="25" customWidth="1"/>
     <col min="2" max="2" width="18" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.08984375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="30.453125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="25" customWidth="1"/>
     <col min="6" max="6" width="20" style="25" customWidth="1"/>
-    <col min="7" max="7" width="24.6328125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="27.453125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="56.453125" style="25" customWidth="1"/>
-    <col min="10" max="10" width="37.6328125" style="25" customWidth="1"/>
-    <col min="11" max="16384" width="8.6328125" style="25"/>
+    <col min="7" max="7" width="24.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="56.42578125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" style="25" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="18" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="18" customFormat="1" ht="15">
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -6464,29 +6470,29 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="40" t="s">
+    <row r="2" spans="2:16" ht="15">
+      <c r="B2" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="9" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="42" t="s">
-        <v>25</v>
+      <c r="J2" s="58" t="s">
+        <v>38</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
@@ -6495,24 +6501,24 @@
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
     </row>
-    <row r="3" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="41"/>
+    <row r="3" spans="2:16" ht="15">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="11" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="43"/>
+        <v>40</v>
+      </c>
+      <c r="I3" s="57"/>
+      <c r="J3" s="59"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="24"/>
@@ -6520,218 +6526,218 @@
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
     </row>
-    <row r="4" spans="2:16" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
+    <row r="4" spans="2:16" s="2" customFormat="1" ht="15">
+      <c r="B4" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="2:16" ht="83.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="83.65" customHeight="1">
       <c r="B5" s="27" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="89" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="92.25">
       <c r="B6" s="28" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="119.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="119.65" customHeight="1">
       <c r="B7" s="30" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E7" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="90">
+      <c r="B8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="29" t="s">
+      <c r="I8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="32" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="8" spans="2:16" ht="72.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="31" t="s">
+    <row r="9" spans="2:16" ht="15">
+      <c r="B9" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="64"/>
+    </row>
+    <row r="10" spans="2:16" s="26" customFormat="1" ht="79.5" customHeight="1">
+      <c r="B10" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="96.75" customHeight="1">
+      <c r="B11" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="H11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>37</v>
+      <c r="I11" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="48"/>
-    </row>
-    <row r="10" spans="2:16" s="26" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+    <row r="12" spans="2:16" ht="33.4" customHeight="1">
+      <c r="B12" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6758,65 +6764,65 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="78.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="61.6328125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="8.6328125" style="5"/>
+    <col min="1" max="1" width="4.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.25" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="45.4" customHeight="1">
       <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="45">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="C6" s="16"/>
     </row>
   </sheetData>
@@ -7178,39 +7184,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{924A4ACD-5488-46C8-ABF3-D5050B19848E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{924A4ACD-5488-46C8-ABF3-D5050B19848E}"/>
 </file>
</xml_diff>